<commit_message>
Pushed the original and submitted versions of the PCB schematic files.
</commit_message>
<xml_diff>
--- a/PCB project budget planning.xlsx
+++ b/PCB project budget planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/dhbsha001_myuct_ac_za/Documents/EEE3088F/PCB design project/PCB planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/dhbsha001_myuct_ac_za/Documents/EEE3088F/PCB design project/Perfectionist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{9F5FE349-849E-4341-A310-1367BF6AC4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E54A9E55-A1BB-4A2F-A88E-9B76C34253AA}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="8_{9F5FE349-849E-4341-A310-1367BF6AC4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{691AFFBE-0CEB-4C89-B73F-AEE5000E20B7}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{283C822C-7316-4009-AE15-2BE23BF5C06F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t>Component</t>
   </si>
@@ -50,33 +50,15 @@
     <t>DC-DC</t>
   </si>
   <si>
-    <t>270k ohm</t>
-  </si>
-  <si>
     <t>150k ohm</t>
   </si>
   <si>
-    <t>3.3M ohm</t>
-  </si>
-  <si>
-    <t>1.5M ohm</t>
-  </si>
-  <si>
-    <t>120k ohm</t>
-  </si>
-  <si>
     <t>10 uF</t>
   </si>
   <si>
     <t>1 uF</t>
   </si>
   <si>
-    <t>22 uF</t>
-  </si>
-  <si>
-    <t>2.2 uH</t>
-  </si>
-  <si>
     <t>INA219</t>
   </si>
   <si>
@@ -98,57 +80,21 @@
     <t>AP2127K-3.3TRG1</t>
   </si>
   <si>
-    <t>RC2512FK-072R2L</t>
-  </si>
-  <si>
     <t>INA219AIDCNR</t>
   </si>
   <si>
-    <t>NR3015T2R2M</t>
-  </si>
-  <si>
-    <t>220k ohm</t>
-  </si>
-  <si>
     <t>Quantity(x2)</t>
   </si>
   <si>
-    <t xml:space="preserve">2.2 ohm </t>
-  </si>
-  <si>
-    <t>0603WAF1203T5E</t>
-  </si>
-  <si>
     <t>0603WAF1503T5E</t>
   </si>
   <si>
-    <t>0603WAF2203T5E</t>
-  </si>
-  <si>
-    <t>0603WAF2703T5E</t>
-  </si>
-  <si>
-    <t>0603WAF1504T5E</t>
-  </si>
-  <si>
-    <t>0603WAF3304T5E</t>
-  </si>
-  <si>
     <t>CL31B105KBHNNNE</t>
   </si>
   <si>
-    <t>CL21A106KAYNNNE</t>
-  </si>
-  <si>
-    <t>CL10A226MQ8NRNC</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>2.2 uF</t>
   </si>
   <si>
@@ -173,9 +119,6 @@
     <t>5V Boost</t>
   </si>
   <si>
-    <t>V1</t>
-  </si>
-  <si>
     <t>Savings over previous</t>
   </si>
   <si>
@@ -188,9 +131,6 @@
     <t>200m ohm 2W shunt</t>
   </si>
   <si>
-    <t>V2</t>
-  </si>
-  <si>
     <t>V3</t>
   </si>
   <si>
@@ -276,6 +216,9 @@
   </si>
   <si>
     <t>step down to 5V</t>
+  </si>
+  <si>
+    <t>DRV8833PWP</t>
   </si>
 </sst>
 </file>
@@ -690,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915D5376-70C8-4982-9CA7-DEFA2243E276}">
-  <dimension ref="B1:N68"/>
+  <dimension ref="B2:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E52" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -709,37 +652,32 @@
     <col min="12" max="12" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -755,12 +693,12 @@
         <v>4.1909999999999998</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -772,16 +710,16 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G17" si="0">3*D4 + F4*E4*2</f>
+        <f t="shared" ref="G4:G13" si="0">3*D4 + F4*E4*2</f>
         <v>3.45</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -796,16 +734,13 @@
         <f t="shared" si="0"/>
         <v>5.8680000000000003</v>
       </c>
-      <c r="H5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -821,13 +756,13 @@
         <v>3.133</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
       <c r="D7">
         <v>1</v>
       </c>
@@ -835,40 +770,40 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>6.6600000000000006E-2</v>
+        <v>0.41849999999999998</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>3.1332</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+        <v>3.8369999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -884,81 +819,75 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F10">
-        <v>1E-3</v>
+        <v>2.24E-2</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
+        <v>0.26879999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
         <v>2E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1E-3</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>3.0019999999999998</v>
-      </c>
-      <c r="H11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1.4E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>3.0028000000000001</v>
-      </c>
-      <c r="H12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -967,386 +896,135 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>1.1999999999999999E-3</v>
+        <v>0.1263</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>3.0024000000000002</v>
-      </c>
-      <c r="H13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+        <v>3.2526000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>2.24E-2</v>
+        <v>0.68</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
-        <v>4.48E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+        <f>3*D14 + F14*E14*2</f>
+        <v>5.7200000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15">
-        <v>9.9000000000000008E-3</v>
+        <v>0.22</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
-        <v>1.9800000000000002E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
+        <f t="shared" ref="G15:G18" si="1">3*D15 + F15*E15*2</f>
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F16">
-        <v>7.1000000000000004E-3</v>
+        <v>2.93E-2</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
-        <v>1.4200000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.2344</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>6.3799999999999996E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
-        <v>3.1276000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="G18" s="2">
-        <f>SUM(G3:G17)</f>
-        <v>31.994999999999994</v>
-      </c>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>0.59550000000000003</v>
-      </c>
-      <c r="G23">
-        <f>3*D23 + F23*E23*2</f>
-        <v>4.1909999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="G24">
-        <f t="shared" ref="G24:G33" si="1">3*D24 + F24*E24*2</f>
-        <v>3.45</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>1.4339999999999999</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="1"/>
-        <v>5.8680000000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>6.6500000000000004E-2</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="1"/>
-        <v>3.133</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>0.41849999999999998</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="1"/>
-        <v>3.8369999999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>6.6600000000000006E-2</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="1"/>
-        <v>3.1332</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="F30">
-        <v>2.24E-2</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="1"/>
-        <v>8.9599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>2E-3</v>
-      </c>
-      <c r="G31">
         <f t="shared" si="1"/>
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G32">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>0.01</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>0.1263</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="1"/>
-        <v>3.2526000000000002</v>
-      </c>
-      <c r="H33" t="s">
-        <v>46</v>
-      </c>
-      <c r="I33" t="s">
-        <v>47</v>
-      </c>
+        <v>0.24</v>
+      </c>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="G19" s="2">
+        <f>SUM(G3:G18)</f>
+        <v>37.603000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="C26" s="1"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="G34" s="2">
-        <f>SUM(G23:G33)</f>
-        <v>26.970600000000001</v>
-      </c>
-      <c r="H34" s="3">
-        <f>G18-G34</f>
-        <v>5.0243999999999929</v>
-      </c>
-      <c r="I34">
-        <f>28.5-G34</f>
-        <v>1.529399999999999</v>
-      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="3"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.45">
@@ -1354,27 +1032,27 @@
         <v>0</v>
       </c>
       <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
         <v>15</v>
       </c>
-      <c r="D37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>24</v>
-      </c>
       <c r="F37" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1395,7 +1073,7 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1416,7 +1094,7 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1434,10 +1112,10 @@
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1455,10 +1133,10 @@
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1476,10 +1154,10 @@
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1497,10 +1175,10 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -1518,10 +1196,10 @@
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1539,10 +1217,10 @@
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -1560,10 +1238,10 @@
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1581,10 +1259,10 @@
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1600,10 +1278,10 @@
         <v>3.2526000000000002</v>
       </c>
       <c r="H48" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="I48" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.45">
@@ -1613,7 +1291,7 @@
       </c>
       <c r="H49" s="3">
         <f>G34-G49</f>
-        <v>3.3199999999997232E-2</v>
+        <v>-26.937400000000004</v>
       </c>
       <c r="I49">
         <f>28.5-G49</f>
@@ -1625,27 +1303,27 @@
         <v>0</v>
       </c>
       <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
         <v>15</v>
       </c>
-      <c r="D51" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51" t="s">
-        <v>24</v>
-      </c>
       <c r="F51" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G51" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -1663,10 +1341,10 @@
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B53" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C53" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -1678,16 +1356,16 @@
         <v>0.22</v>
       </c>
       <c r="G53">
-        <f t="shared" ref="G53:G80" si="3">3*D53 + F53*E53*2</f>
+        <f t="shared" ref="G53:G65" si="3">3*D53 + F53*E53*2</f>
         <v>3.88</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -1705,10 +1383,10 @@
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -1726,10 +1404,10 @@
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -1747,10 +1425,10 @@
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -1768,10 +1446,10 @@
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B58" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -1789,10 +1467,10 @@
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -1810,10 +1488,10 @@
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C60" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -1831,10 +1509,10 @@
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -1850,18 +1528,18 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I61" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="J61" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -1879,10 +1557,10 @@
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -1900,10 +1578,10 @@
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B64" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C64" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -1921,10 +1599,10 @@
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -1948,7 +1626,7 @@
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F68" s="5" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="G68" s="5">
         <f>G66+G49</f>

</xml_diff>